<commit_message>
changes to master spreedsheet
</commit_message>
<xml_diff>
--- a/data/RNAseq-cellline-master.xlsx
+++ b/data/RNAseq-cellline-master.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14260" tabRatio="500"/>
+    <workbookView xWindow="25440" yWindow="0" windowWidth="25120" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Library information" sheetId="1" r:id="rId1"/>
     <sheet name="NEBNext index information" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Library information'!$A$1:$O$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Library information'!$A$1:$O$39</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -1176,7 +1176,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1189,6 +1189,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1301,7 +1315,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="50">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1319,6 +1333,13 @@
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1336,6 +1357,13 @@
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="11"/>
   </cellStyles>
@@ -1669,7 +1697,7 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
tracking master spreedsheet changes
</commit_message>
<xml_diff>
--- a/data/RNAseq-cellline-master.xlsx
+++ b/data/RNAseq-cellline-master.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25720" yWindow="240" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="13400" yWindow="0" windowWidth="25360" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Library information" sheetId="1" r:id="rId1"/>
@@ -1737,16 +1737,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7" style="7" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="8" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
@@ -1769,7 +1769,7 @@
     <col min="22" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1" ht="45">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="45">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:21">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:21">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="19" customFormat="1">
+    <row r="4" spans="1:21" s="19" customFormat="1">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -1991,8 +1991,11 @@
       <c r="R4" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" s="19" customFormat="1">
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+    </row>
+    <row r="5" spans="1:21" s="19" customFormat="1">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -2044,8 +2047,11 @@
       <c r="R5" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:21">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -2150,8 +2156,11 @@
       <c r="R7" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" s="19" customFormat="1">
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+    </row>
+    <row r="8" spans="1:21" s="19" customFormat="1">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -2203,8 +2212,11 @@
       <c r="R8" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" s="19" customFormat="1">
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+    </row>
+    <row r="9" spans="1:21" s="19" customFormat="1">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -2256,8 +2268,11 @@
       <c r="R9" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" s="19" customFormat="1">
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" spans="1:21" s="19" customFormat="1">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -2311,7 +2326,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="19" customFormat="1">
+    <row r="11" spans="1:21" s="19" customFormat="1">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -2365,7 +2380,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="19" customFormat="1">
+    <row r="12" spans="1:21" s="19" customFormat="1">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -2418,8 +2433,11 @@
       <c r="R12" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" s="19" customFormat="1">
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" spans="1:21" s="19" customFormat="1">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -2472,8 +2490,11 @@
       <c r="R13" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -2526,9 +2547,8 @@
       <c r="R14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="S14" s="19"/>
-    </row>
-    <row r="15" spans="1:19">
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -2581,8 +2601,9 @@
       <c r="R15" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="S15" s="19"/>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -2640,7 +2661,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:21">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -2698,7 +2719,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:21">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -2755,7 +2776,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:21">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -2812,8 +2833,10 @@
       <c r="R19" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:19">
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -2866,8 +2889,9 @@
       <c r="R20" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="S20" s="19"/>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -2921,7 +2945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:21">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -2974,7 +2998,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:21">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -3026,9 +3050,8 @@
       <c r="R23" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="S23" s="19"/>
-    </row>
-    <row r="24" spans="1:19">
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -3086,7 +3109,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:21">
       <c r="A25" s="14">
         <v>24</v>
       </c>
@@ -3144,7 +3167,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:21">
       <c r="A26" s="14">
         <v>25</v>
       </c>
@@ -3197,8 +3220,11 @@
       <c r="R26" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:19">
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" s="14">
         <v>26</v>
       </c>
@@ -3251,8 +3277,11 @@
       <c r="R27" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:19">
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" s="14">
         <v>27</v>
       </c>
@@ -3306,7 +3335,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="19" customFormat="1">
+    <row r="29" spans="1:21" s="19" customFormat="1">
       <c r="A29" s="14">
         <v>28</v>
       </c>
@@ -3360,8 +3389,10 @@
         <v>36</v>
       </c>
       <c r="S29" s="7"/>
-    </row>
-    <row r="30" spans="1:19">
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" s="14">
         <v>29</v>
       </c>
@@ -3413,8 +3444,11 @@
       <c r="R30" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:19">
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" s="14">
         <v>30</v>
       </c>
@@ -3467,8 +3501,11 @@
       <c r="R31" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" s="19" customFormat="1">
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+    </row>
+    <row r="32" spans="1:21" s="19" customFormat="1">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -3521,8 +3558,11 @@
       <c r="R32" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" s="19" customFormat="1">
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+    </row>
+    <row r="33" spans="1:21" s="19" customFormat="1">
       <c r="A33" s="19">
         <v>32</v>
       </c>
@@ -3575,8 +3615,11 @@
       <c r="R33" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:18">
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" s="14">
         <v>33</v>
       </c>
@@ -3633,8 +3676,11 @@
       <c r="R34" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:18">
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" s="14">
         <v>34</v>
       </c>
@@ -3691,8 +3737,11 @@
       <c r="R35" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:18">
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" s="14">
         <v>35</v>
       </c>
@@ -3745,8 +3794,11 @@
       <c r="R36" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:18">
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" s="14">
         <v>36</v>
       </c>
@@ -3799,8 +3851,11 @@
       <c r="R37" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:18">
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" s="14">
         <v>37</v>
       </c>
@@ -3849,7 +3904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:18" s="19" customFormat="1">
+    <row r="39" spans="1:21" s="19" customFormat="1">
       <c r="A39" s="14">
         <v>38</v>
       </c>
@@ -3902,8 +3957,11 @@
       <c r="R39" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:18">
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+    </row>
+    <row r="40" spans="1:21">
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -3917,7 +3975,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:S49">
+  <sortState ref="A2:U49">
     <sortCondition ref="A2:A49"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
added groups for pooling prior to dropoff at NGSC
</commit_message>
<xml_diff>
--- a/data/RNAseq-cellline-master.xlsx
+++ b/data/RNAseq-cellline-master.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="0" windowWidth="25360" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="-460" windowWidth="23040" windowHeight="17280" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Library information" sheetId="1" r:id="rId1"/>
     <sheet name="NEBNext index information" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Library information'!$A$1:$O$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Library information'!$A$12:$O$39</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="210">
   <si>
     <t>Library Prep #</t>
   </si>
@@ -92,9 +93,6 @@
   </si>
   <si>
     <t>n/a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEQUENCE Date </t>
   </si>
   <si>
     <t>RNA starting vol.</t>
@@ -1022,6 +1020,96 @@
   </si>
   <si>
     <t>but</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEQUENCE Date/group </t>
+  </si>
+  <si>
+    <t>PD6419_C5_BULK</t>
+  </si>
+  <si>
+    <t>PD6555_C3_YFP</t>
+  </si>
+  <si>
+    <t>PD2838_C3_YFP</t>
+  </si>
+  <si>
+    <t>PD6421_C2_YFP</t>
+  </si>
+  <si>
+    <t>PD6556_C3_BULK</t>
+  </si>
+  <si>
+    <t>PD6499_C3_YFP</t>
+  </si>
+  <si>
+    <t>PD6694_C2_YFP</t>
+  </si>
+  <si>
+    <t>PD7160_C5_BULK</t>
+  </si>
+  <si>
+    <t>PD7160_C5_YFP</t>
+  </si>
+  <si>
+    <t>PD7160_C2_YFP</t>
+  </si>
+  <si>
+    <t>PD6556_C4_BULK</t>
+  </si>
+  <si>
+    <t>PD6556_C3_YFP</t>
+  </si>
+  <si>
+    <t>PD6499_C3_BULK</t>
+  </si>
+  <si>
+    <t>PD6694_C2_BULK</t>
+  </si>
+  <si>
+    <t>PD7160_C2_BULK</t>
+  </si>
+  <si>
+    <t>PD6422_C1_BULK</t>
+  </si>
+  <si>
+    <t>PD6422_C1_YFP</t>
+  </si>
+  <si>
+    <t>PD2838_C3_BULK</t>
+  </si>
+  <si>
+    <t>PD6883_C4_BULK</t>
+  </si>
+  <si>
+    <t>PD6883_C4_YFP</t>
+  </si>
+  <si>
+    <t>PD6419_C5_YFP</t>
+  </si>
+  <si>
+    <t>PD6556_C5_YFP</t>
+  </si>
+  <si>
+    <t>PD6555_C3_BULK</t>
+  </si>
+  <si>
+    <t>PD6883_C1_YFP</t>
+  </si>
+  <si>
+    <t>PD6421_C2_BULK</t>
+  </si>
+  <si>
+    <t>PD2699_C4_2_BULK</t>
+  </si>
+  <si>
+    <t>PD2699_C4_2_YFP</t>
+  </si>
+  <si>
+    <t>PD6883_C1_BULK</t>
+  </si>
+  <si>
+    <t>SEQUENCE GROUP ID</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1264,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="58">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1235,8 +1323,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1322,35 +1414,8 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="58">
+  <cellStyles count="62">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1379,6 +1444,8 @@
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1407,6 +1474,8 @@
     <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="11"/>
   </cellStyles>
@@ -1739,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O29" sqref="A1:O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1759,7 +1828,7 @@
     <col min="12" max="12" width="7.33203125" style="9" customWidth="1"/>
     <col min="13" max="13" width="8.1640625" style="7" customWidth="1"/>
     <col min="14" max="14" width="7.83203125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" style="7" customWidth="1"/>
     <col min="16" max="16" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.1640625" style="7" customWidth="1"/>
     <col min="18" max="18" width="67.5" style="7" bestFit="1" customWidth="1"/>
@@ -1780,7 +1849,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>3</v>
@@ -1801,19 +1870,19 @@
         <v>9</v>
       </c>
       <c r="K1" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="N1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>35</v>
-      </c>
       <c r="O1" s="21" t="s">
-        <v>23</v>
+        <v>180</v>
       </c>
       <c r="P1" s="21" t="s">
         <v>6</v>
@@ -1827,225 +1896,229 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="14">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C2" s="14">
-        <v>142</v>
+        <v>212</v>
       </c>
       <c r="D2" s="15">
-        <v>4.4000000000000004</v>
+        <f>1000/C2</f>
+        <v>4.716981132075472</v>
       </c>
       <c r="E2" s="16">
         <f>D2*C2</f>
-        <v>624.80000000000007</v>
+        <v>1000.0000000000001</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G2" s="25">
-        <v>42620</v>
+        <v>42621</v>
       </c>
       <c r="H2" s="18">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="27">
-        <v>357</v>
+        <v>325</v>
       </c>
       <c r="L2" s="15">
-        <v>60.72</v>
+        <v>21.74</v>
       </c>
       <c r="M2" s="15">
         <f>((L2)/((K2*607.4)+157.9)*1000000)</f>
-        <v>279.81605504523742</v>
-      </c>
-      <c r="N2" s="28">
+        <v>110.04090342873079</v>
+      </c>
+      <c r="N2" s="15">
         <f>M2/4</f>
-        <v>69.954013761309355</v>
-      </c>
-      <c r="O2" s="17">
-        <v>42641</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>27.510225857182697</v>
+      </c>
+      <c r="O2" s="18">
+        <v>1</v>
+      </c>
+      <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
       <c r="R2" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="14">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C3" s="14">
-        <v>580</v>
+        <v>420</v>
       </c>
       <c r="D3" s="15">
-        <v>1.72</v>
+        <f>1000/C3</f>
+        <v>2.3809523809523809</v>
       </c>
       <c r="E3" s="16">
         <f>D3*C3</f>
-        <v>997.6</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="25">
-        <v>42620</v>
+        <v>42621</v>
       </c>
       <c r="H3" s="18">
-        <v>3</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>75</v>
+        <v>12</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>163</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" s="27">
-        <v>379</v>
+        <v>325</v>
       </c>
       <c r="L3" s="15">
-        <v>29.62</v>
+        <v>17.61</v>
       </c>
       <c r="M3" s="15">
         <f>((L3)/((K3*607.4)+157.9)*1000000)</f>
-        <v>128.57995550491074</v>
-      </c>
-      <c r="N3" s="28">
+        <v>89.13616878472628</v>
+      </c>
+      <c r="N3" s="15">
         <f>M3/4</f>
-        <v>32.144988876227686</v>
-      </c>
-      <c r="O3" s="17">
-        <v>42641</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>22.28404219618157</v>
+      </c>
+      <c r="O3" s="18">
+        <v>1</v>
+      </c>
+      <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
       <c r="R3" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="19" customFormat="1">
-      <c r="A4" s="19">
-        <v>3</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="19">
-        <v>252</v>
-      </c>
-      <c r="D4" s="31">
-        <v>3.97</v>
-      </c>
-      <c r="E4" s="32">
+      <c r="A4" s="14">
+        <v>22</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="14">
+        <v>342</v>
+      </c>
+      <c r="D4" s="15">
+        <f>1000/C4</f>
+        <v>2.9239766081871346</v>
+      </c>
+      <c r="E4" s="16">
         <f>D4*C4</f>
-        <v>1000.44</v>
-      </c>
-      <c r="F4" s="32" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="33">
-        <v>42629</v>
-      </c>
-      <c r="H4" s="29">
+      <c r="G4" s="17">
+        <v>42622</v>
+      </c>
+      <c r="H4" s="18">
         <v>18</v>
       </c>
-      <c r="I4" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="35">
-        <v>355</v>
-      </c>
-      <c r="L4" s="31">
-        <v>23.27</v>
-      </c>
-      <c r="M4" s="31">
+      <c r="I4" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="27">
+        <v>369</v>
+      </c>
+      <c r="L4" s="15">
+        <v>21.7</v>
+      </c>
+      <c r="M4" s="15">
         <f>((L4)/((K4*607.4)+157.9)*1000000)</f>
-        <v>107.8388710238761</v>
-      </c>
-      <c r="N4" s="31">
+        <v>96.750390679860971</v>
+      </c>
+      <c r="N4" s="15">
         <f>M4/4</f>
-        <v>26.959717755969024</v>
-      </c>
-      <c r="O4" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R4" s="19" t="s">
-        <v>36</v>
+        <v>24.187597669965243</v>
+      </c>
+      <c r="O4" s="18">
+        <v>1</v>
+      </c>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
     <row r="5" spans="1:21" s="19" customFormat="1">
-      <c r="A5" s="19">
-        <v>4</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="19">
-        <v>226</v>
-      </c>
-      <c r="D5" s="31">
-        <v>3</v>
-      </c>
-      <c r="E5" s="32">
+      <c r="A5" s="14">
+        <v>25</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="14">
+        <v>136</v>
+      </c>
+      <c r="D5" s="15">
+        <f>1000/C5</f>
+        <v>7.3529411764705879</v>
+      </c>
+      <c r="E5" s="16">
         <f>D5*C5</f>
-        <v>678</v>
-      </c>
-      <c r="F5" s="32" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="33">
-        <v>42620</v>
-      </c>
-      <c r="H5" s="29">
+      <c r="G5" s="17">
+        <v>42625</v>
+      </c>
+      <c r="H5" s="18">
         <v>2</v>
       </c>
-      <c r="I5" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="35">
-        <v>379</v>
-      </c>
-      <c r="L5" s="31">
-        <v>54.6</v>
-      </c>
-      <c r="M5" s="31">
+      <c r="I5" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="27">
+        <v>326</v>
+      </c>
+      <c r="L5" s="15">
+        <v>15.14</v>
+      </c>
+      <c r="M5" s="15">
         <f>((L5)/((K5*607.4)+157.9)*1000000)</f>
-        <v>237.01774377340064</v>
-      </c>
-      <c r="N5" s="37">
+        <v>76.398935662912166</v>
+      </c>
+      <c r="N5" s="15">
         <f>M5/4</f>
-        <v>59.25443594335016</v>
-      </c>
-      <c r="O5" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R5" s="19" t="s">
-        <v>36</v>
+        <v>19.099733915728041</v>
+      </c>
+      <c r="O5" s="18">
+        <v>1</v>
+      </c>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
@@ -2053,442 +2126,458 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="14">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C6" s="14">
-        <v>34</v>
+        <v>294</v>
       </c>
       <c r="D6" s="15">
-        <v>4.3</v>
+        <f>1000/C6</f>
+        <v>3.4013605442176869</v>
       </c>
       <c r="E6" s="16">
         <f>D6*C6</f>
-        <v>146.19999999999999</v>
+        <v>999.99999999999989</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="25">
-        <v>42620</v>
+      <c r="G6" s="17">
+        <v>42625</v>
       </c>
       <c r="H6" s="18">
-        <v>4</v>
-      </c>
-      <c r="I6" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>31</v>
+        <v>5</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="K6" s="27">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="L6" s="15">
-        <v>41.84</v>
+        <v>45.06</v>
       </c>
       <c r="M6" s="15">
         <f>((L6)/((K6*607.4)+157.9)*1000000)</f>
-        <v>194.44412171346914</v>
-      </c>
-      <c r="N6" s="28">
+        <v>211.79997546391763</v>
+      </c>
+      <c r="N6" s="15">
         <f>M6/4</f>
-        <v>48.611030428367286</v>
-      </c>
-      <c r="O6" s="14"/>
+        <v>52.949993865979408</v>
+      </c>
+      <c r="O6" s="18">
+        <v>1</v>
+      </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
       <c r="R6" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="14">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C7" s="14">
-        <v>296</v>
+        <v>352</v>
       </c>
       <c r="D7" s="15">
-        <v>3.38</v>
+        <f>1000/C7</f>
+        <v>2.8409090909090908</v>
       </c>
       <c r="E7" s="16">
         <f>D7*C7</f>
-        <v>1000.48</v>
+        <v>1000</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="25">
-        <v>42620</v>
+      <c r="G7" s="17">
+        <v>42625</v>
       </c>
       <c r="H7" s="18">
-        <v>5</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="K7" s="27">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="L7" s="15">
-        <v>23</v>
+        <v>45.18</v>
       </c>
       <c r="M7" s="15">
         <f>((L7)/((K7*607.4)+157.9)*1000000)</f>
-        <v>105.40087849340901</v>
-      </c>
-      <c r="N7" s="28">
+        <v>212.36402333466043</v>
+      </c>
+      <c r="N7" s="15">
         <f>M7/4</f>
-        <v>26.350219623352253</v>
-      </c>
-      <c r="O7" s="14"/>
+        <v>53.091005833665108</v>
+      </c>
+      <c r="O7" s="18">
+        <v>1</v>
+      </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
       <c r="R7" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S7" s="19"/>
       <c r="T7" s="19"/>
       <c r="U7" s="19"/>
     </row>
     <row r="8" spans="1:21" s="19" customFormat="1">
-      <c r="A8" s="19">
-        <v>7</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="19">
-        <v>65</v>
-      </c>
-      <c r="D8" s="31">
-        <v>5</v>
-      </c>
-      <c r="E8" s="32">
+      <c r="A8" s="14">
+        <v>38</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="14">
+        <v>290</v>
+      </c>
+      <c r="D8" s="15">
+        <f>1000/C8</f>
+        <v>3.4482758620689653</v>
+      </c>
+      <c r="E8" s="16">
         <f>D8*C8</f>
-        <v>325</v>
-      </c>
-      <c r="F8" s="32" t="s">
+        <v>999.99999999999989</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="33">
-        <v>42620</v>
-      </c>
-      <c r="H8" s="29">
-        <v>7</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="35">
-        <v>372</v>
-      </c>
-      <c r="L8" s="31">
-        <v>49.02</v>
-      </c>
-      <c r="M8" s="31">
+      <c r="G8" s="17">
+        <v>42626</v>
+      </c>
+      <c r="H8" s="18">
+        <v>1</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="27">
+        <v>326</v>
+      </c>
+      <c r="L8" s="15">
+        <v>29.92</v>
+      </c>
+      <c r="M8" s="15">
         <f>((L8)/((K8*607.4)+157.9)*1000000)</f>
-        <v>216.79646297145604</v>
-      </c>
-      <c r="N8" s="37">
+        <v>150.98125198377357</v>
+      </c>
+      <c r="N8" s="15">
         <f>M8/4</f>
-        <v>54.199115742864009</v>
-      </c>
-      <c r="O8" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R8" s="19" t="s">
-        <v>36</v>
+        <v>37.745312995943394</v>
+      </c>
+      <c r="O8" s="18">
+        <v>1</v>
+      </c>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
     </row>
     <row r="9" spans="1:21" s="19" customFormat="1">
-      <c r="A9" s="19">
-        <v>8</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="19">
-        <v>308</v>
-      </c>
-      <c r="D9" s="31">
+      <c r="A9" s="14">
         <v>4</v>
       </c>
-      <c r="E9" s="32">
+      <c r="B9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14">
+        <v>226</v>
+      </c>
+      <c r="D9" s="15">
+        <v>3</v>
+      </c>
+      <c r="E9" s="16">
         <f>D9*C9</f>
-        <v>1232</v>
-      </c>
-      <c r="F9" s="32" t="s">
+        <v>678</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="25">
         <v>42620</v>
       </c>
-      <c r="H9" s="29">
-        <v>14</v>
-      </c>
-      <c r="I9" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="J9" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="35">
-        <v>363</v>
-      </c>
-      <c r="L9" s="31">
-        <v>16.03</v>
-      </c>
-      <c r="M9" s="31">
+      <c r="H9" s="18">
+        <v>2</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="27">
+        <v>379</v>
+      </c>
+      <c r="L9" s="15">
+        <v>54.6</v>
+      </c>
+      <c r="M9" s="15">
         <f>((L9)/((K9*607.4)+157.9)*1000000)</f>
-        <v>72.650934242066768</v>
-      </c>
-      <c r="N9" s="37">
+        <v>237.01774377340064</v>
+      </c>
+      <c r="N9" s="28">
         <f>M9/4</f>
-        <v>18.162733560516692</v>
-      </c>
-      <c r="O9" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R9" s="19" t="s">
-        <v>36</v>
+        <v>59.25443594335016</v>
+      </c>
+      <c r="O9" s="18">
+        <v>2</v>
+      </c>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
     </row>
     <row r="10" spans="1:21" s="19" customFormat="1">
-      <c r="A10" s="19">
-        <v>9</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="19">
-        <v>212</v>
-      </c>
-      <c r="D10" s="31">
-        <f>1000/C10</f>
-        <v>4.716981132075472</v>
-      </c>
-      <c r="E10" s="32">
+      <c r="A10" s="14">
+        <v>5</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="14">
+        <v>34</v>
+      </c>
+      <c r="D10" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="E10" s="16">
         <f>D10*C10</f>
-        <v>1000.0000000000001</v>
-      </c>
-      <c r="F10" s="32" t="s">
+        <v>146.19999999999999</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="33">
-        <v>42621</v>
-      </c>
-      <c r="H10" s="29">
-        <v>10</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="J10" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" s="35">
-        <v>325</v>
-      </c>
-      <c r="L10" s="31">
-        <v>21.74</v>
-      </c>
-      <c r="M10" s="31">
+      <c r="G10" s="25">
+        <v>42620</v>
+      </c>
+      <c r="H10" s="18">
+        <v>4</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="27">
+        <v>354</v>
+      </c>
+      <c r="L10" s="15">
+        <v>41.84</v>
+      </c>
+      <c r="M10" s="15">
         <f>((L10)/((K10*607.4)+157.9)*1000000)</f>
-        <v>110.04090342873079</v>
-      </c>
-      <c r="N10" s="31">
+        <v>194.44412171346914</v>
+      </c>
+      <c r="N10" s="28">
         <f>M10/4</f>
-        <v>27.510225857182697</v>
-      </c>
-      <c r="O10" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R10" s="19" t="s">
-        <v>36</v>
+        <v>48.611030428367286</v>
+      </c>
+      <c r="O10" s="18">
+        <v>2</v>
+      </c>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="19" customFormat="1">
-      <c r="A11" s="19">
-        <v>10</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="19">
-        <v>252</v>
-      </c>
-      <c r="D11" s="31">
-        <f>1000/C11</f>
-        <v>3.9682539682539684</v>
-      </c>
-      <c r="E11" s="32">
+      <c r="A11" s="14">
+        <v>6</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="14">
+        <v>296</v>
+      </c>
+      <c r="D11" s="15">
+        <v>3.38</v>
+      </c>
+      <c r="E11" s="16">
         <f>D11*C11</f>
-        <v>1000</v>
-      </c>
-      <c r="F11" s="32" t="s">
+        <v>1000.48</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="33">
-        <v>42621</v>
-      </c>
-      <c r="H11" s="29">
-        <v>11</v>
-      </c>
-      <c r="I11" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="J11" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" s="35">
-        <v>325</v>
-      </c>
-      <c r="L11" s="31">
-        <v>18.64</v>
-      </c>
-      <c r="M11" s="31">
+      <c r="G11" s="25">
+        <v>42620</v>
+      </c>
+      <c r="H11" s="18">
+        <v>5</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="27">
+        <v>359</v>
+      </c>
+      <c r="L11" s="15">
+        <v>23</v>
+      </c>
+      <c r="M11" s="15">
         <f>((L11)/((K11*607.4)+157.9)*1000000)</f>
-        <v>94.349698248001019</v>
-      </c>
-      <c r="N11" s="31">
+        <v>105.40087849340901</v>
+      </c>
+      <c r="N11" s="28">
         <f>M11/4</f>
-        <v>23.587424562000255</v>
-      </c>
-      <c r="O11" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R11" s="19" t="s">
-        <v>36</v>
+        <v>26.350219623352253</v>
+      </c>
+      <c r="O11" s="18">
+        <v>2</v>
+      </c>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="19" customFormat="1">
-      <c r="A12" s="19">
-        <v>11</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="19">
-        <v>288</v>
-      </c>
-      <c r="D12" s="31">
-        <f>1000/C12</f>
-        <v>3.4722222222222223</v>
-      </c>
-      <c r="E12" s="32">
+      <c r="A12" s="14">
+        <v>8</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="14">
+        <v>308</v>
+      </c>
+      <c r="D12" s="15">
+        <v>4</v>
+      </c>
+      <c r="E12" s="16">
         <f>D12*C12</f>
-        <v>1000</v>
-      </c>
-      <c r="F12" s="32" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="33">
-        <v>42621</v>
-      </c>
-      <c r="H12" s="29">
-        <v>21</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="J12" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="K12" s="35">
-        <v>325</v>
-      </c>
-      <c r="L12" s="31">
-        <v>24.09</v>
-      </c>
-      <c r="M12" s="31">
+      <c r="G12" s="25">
+        <v>42620</v>
+      </c>
+      <c r="H12" s="18">
+        <v>14</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="27">
+        <v>363</v>
+      </c>
+      <c r="L12" s="15">
+        <v>16.03</v>
+      </c>
+      <c r="M12" s="15">
         <f>((L12)/((K12*607.4)+157.9)*1000000)</f>
-        <v>121.93584929154208</v>
-      </c>
-      <c r="N12" s="31">
+        <v>72.650934242066768</v>
+      </c>
+      <c r="N12" s="28">
         <f>M12/4</f>
-        <v>30.483962322885521</v>
-      </c>
-      <c r="O12" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R12" s="19" t="s">
-        <v>36</v>
+        <v>18.162733560516692</v>
+      </c>
+      <c r="O12" s="18">
+        <v>2</v>
+      </c>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
     </row>
     <row r="13" spans="1:21" s="19" customFormat="1">
-      <c r="A13" s="19">
-        <v>12</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="19">
-        <v>240</v>
-      </c>
-      <c r="D13" s="31">
+      <c r="A13" s="14">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="14">
+        <v>288</v>
+      </c>
+      <c r="D13" s="15">
         <f>1000/C13</f>
-        <v>4.166666666666667</v>
-      </c>
-      <c r="E13" s="32">
+        <v>3.4722222222222223</v>
+      </c>
+      <c r="E13" s="16">
         <f>D13*C13</f>
-        <v>1000.0000000000001</v>
-      </c>
-      <c r="F13" s="32" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="25">
         <v>42621</v>
       </c>
-      <c r="H13" s="29">
-        <v>9</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="J13" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="35">
+      <c r="H13" s="18">
+        <v>21</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="27">
         <v>325</v>
       </c>
-      <c r="L13" s="31">
-        <v>18.850000000000001</v>
-      </c>
-      <c r="M13" s="31">
+      <c r="L13" s="15">
+        <v>24.09</v>
+      </c>
+      <c r="M13" s="15">
         <f>((L13)/((K13*607.4)+157.9)*1000000)</f>
-        <v>95.412650857018207</v>
-      </c>
-      <c r="N13" s="31">
+        <v>121.93584929154208</v>
+      </c>
+      <c r="N13" s="15">
         <f>M13/4</f>
-        <v>23.853162714254552</v>
-      </c>
-      <c r="O13" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R13" s="19" t="s">
-        <v>36</v>
+        <v>30.483962322885521</v>
+      </c>
+      <c r="O13" s="18">
+        <v>2</v>
+      </c>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
@@ -2496,17 +2585,17 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="14">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C14" s="14">
-        <v>196</v>
+        <v>284</v>
       </c>
       <c r="D14" s="15">
         <f>1000/C14</f>
-        <v>5.1020408163265305</v>
+        <v>3.5211267605633805</v>
       </c>
       <c r="E14" s="16">
         <f>D14*C14</f>
@@ -2515,52 +2604,57 @@
       <c r="F14" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="25">
-        <v>42621</v>
+      <c r="G14" s="17">
+        <v>42625</v>
       </c>
       <c r="H14" s="18">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>31</v>
+        <v>175</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="K14" s="27">
-        <v>325</v>
+        <v>350</v>
       </c>
       <c r="L14" s="15">
-        <v>20.02</v>
+        <v>83.06</v>
       </c>
       <c r="M14" s="15">
         <f>((L14)/((K14*607.4)+157.9)*1000000)</f>
-        <v>101.33481539297105</v>
+        <v>390.41513453246779</v>
       </c>
       <c r="N14" s="15">
         <f>M14/4</f>
-        <v>25.333703848242763</v>
-      </c>
-      <c r="O14" s="14"/>
+        <v>97.603783633116947</v>
+      </c>
+      <c r="O14" s="18">
+        <v>2</v>
+      </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
       <c r="R14" s="14" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="14">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C15" s="14">
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="D15" s="15">
         <f>1000/C15</f>
-        <v>2.3809523809523809</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="E15" s="16">
         <f>D15*C15</f>
@@ -2569,172 +2663,171 @@
       <c r="F15" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="25">
-        <v>42621</v>
+      <c r="G15" s="17">
+        <v>42626</v>
       </c>
       <c r="H15" s="18">
         <v>12</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>31</v>
+        <v>163</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="K15" s="27">
-        <v>325</v>
+        <v>350</v>
       </c>
       <c r="L15" s="15">
-        <v>17.61</v>
+        <v>140</v>
       </c>
       <c r="M15" s="15">
         <f>((L15)/((K15*607.4)+157.9)*1000000)</f>
-        <v>89.13616878472628</v>
+        <v>658.05584919992157</v>
       </c>
       <c r="N15" s="15">
         <f>M15/4</f>
-        <v>22.28404219618157</v>
-      </c>
-      <c r="O15" s="14"/>
+        <v>164.51396229998039</v>
+      </c>
+      <c r="O15" s="18">
+        <v>2</v>
+      </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S15" s="19"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="14">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C16" s="14">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="D16" s="15">
-        <f>1000/C16</f>
-        <v>4.4642857142857144</v>
+        <v>3.97</v>
       </c>
       <c r="E16" s="16">
         <f>D16*C16</f>
-        <v>1000</v>
+        <v>1000.44</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="25">
-        <v>42621</v>
+        <v>42629</v>
       </c>
       <c r="H16" s="18">
-        <v>14</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>31</v>
+        <v>18</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="K16" s="27">
-        <v>325</v>
+        <v>355</v>
       </c>
       <c r="L16" s="15">
-        <v>19.32</v>
+        <v>23.27</v>
       </c>
       <c r="M16" s="15">
         <f>((L16)/((K16*607.4)+157.9)*1000000)</f>
-        <v>97.791640029580449</v>
+        <v>107.8388710238761</v>
       </c>
       <c r="N16" s="15">
         <f>M16/4</f>
-        <v>24.447910007395112</v>
-      </c>
-      <c r="O16" s="17">
-        <v>42641</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>26.959717755969024</v>
+      </c>
+      <c r="O16" s="18">
+        <v>3</v>
+      </c>
+      <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="14">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C17" s="14">
-        <v>356</v>
+        <v>65</v>
       </c>
       <c r="D17" s="15">
-        <f>1000/C17</f>
-        <v>2.808988764044944</v>
+        <v>5</v>
       </c>
       <c r="E17" s="16">
         <f>D17*C17</f>
-        <v>1000.0000000000001</v>
+        <v>325</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="25">
-        <v>42621</v>
+        <v>42620</v>
       </c>
       <c r="H17" s="18">
-        <v>18</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>131</v>
+        <v>7</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K17" s="27">
-        <v>325</v>
+        <v>372</v>
       </c>
       <c r="L17" s="15">
-        <v>15</v>
+        <v>49.02</v>
       </c>
       <c r="M17" s="15">
         <f>((L17)/((K17*607.4)+157.9)*1000000)</f>
-        <v>75.925186358369913</v>
-      </c>
-      <c r="N17" s="15">
+        <v>216.79646297145604</v>
+      </c>
+      <c r="N17" s="28">
         <f>M17/4</f>
-        <v>18.981296589592478</v>
-      </c>
-      <c r="O17" s="17">
-        <v>42641</v>
-      </c>
-      <c r="P17" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>54.199115742864009</v>
+      </c>
+      <c r="O17" s="18">
+        <v>3</v>
+      </c>
+      <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="14" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="14">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" s="14">
-        <v>10.199999999999999</v>
+        <v>228</v>
       </c>
       <c r="D18" s="15">
-        <v>5</v>
+        <f>1000/C18</f>
+        <v>4.3859649122807021</v>
       </c>
       <c r="E18" s="16">
         <f>D18*C18</f>
-        <v>51</v>
+        <v>1000.0000000000001</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>22</v>
@@ -2743,56 +2836,54 @@
         <v>42622</v>
       </c>
       <c r="H18" s="18">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="K18" s="27">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="L18" s="15">
-        <v>17</v>
+        <v>54.58</v>
       </c>
       <c r="M18" s="15">
         <f>((L18)/((K18*607.4)+157.9)*1000000)</f>
-        <v>75.386923384269764</v>
+        <v>240.09624965083106</v>
       </c>
       <c r="N18" s="15">
         <f>M18/4</f>
-        <v>18.846730846067441</v>
-      </c>
-      <c r="O18" s="17">
-        <v>42641</v>
-      </c>
-      <c r="P18" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>60.024062412707764</v>
+      </c>
+      <c r="O18" s="18">
+        <v>3</v>
+      </c>
+      <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="14">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="14">
-        <v>236</v>
+        <v>268</v>
       </c>
       <c r="D19" s="15">
         <f>1000/C19</f>
-        <v>4.2372881355932206</v>
+        <v>3.7313432835820897</v>
       </c>
       <c r="E19" s="16">
         <f>D19*C19</f>
-        <v>1000.0000000000001</v>
+        <v>1000</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>22</v>
@@ -2801,58 +2892,55 @@
         <v>42622</v>
       </c>
       <c r="H19" s="18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>167</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="K19" s="27">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="L19" s="15">
-        <v>24.46</v>
+        <v>39.69</v>
       </c>
       <c r="M19" s="15">
         <f>((L19)/((K19*607.4)+157.9)*1000000)</f>
-        <v>111.47098404816495</v>
+        <v>178.40904442605463</v>
       </c>
       <c r="N19" s="15">
         <f>M19/4</f>
-        <v>27.867746012041238</v>
-      </c>
-      <c r="O19" s="17">
-        <v>42641</v>
-      </c>
-      <c r="P19" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>44.602261106513659</v>
+      </c>
+      <c r="O19" s="18">
+        <v>3</v>
+      </c>
+      <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
       <c r="R19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
+        <v>35</v>
+      </c>
+      <c r="S19" s="19"/>
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="14">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20" s="14">
-        <v>228</v>
+        <v>392</v>
       </c>
       <c r="D20" s="15">
         <f>1000/C20</f>
-        <v>4.3859649122807021</v>
+        <v>2.5510204081632653</v>
       </c>
       <c r="E20" s="16">
         <f>D20*C20</f>
-        <v>1000.0000000000001</v>
+        <v>1000</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>22</v>
@@ -2861,49 +2949,50 @@
         <v>42622</v>
       </c>
       <c r="H20" s="18">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="K20" s="27">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="L20" s="15">
-        <v>54.58</v>
+        <v>16.190000000000001</v>
       </c>
       <c r="M20" s="15">
         <f>((L20)/((K20*607.4)+157.9)*1000000)</f>
-        <v>240.09624965083106</v>
+        <v>76.099458561048081</v>
       </c>
       <c r="N20" s="15">
         <f>M20/4</f>
-        <v>60.024062412707764</v>
-      </c>
-      <c r="O20" s="17"/>
+        <v>19.02486464026202</v>
+      </c>
+      <c r="O20" s="18">
+        <v>3</v>
+      </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
       <c r="R20" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S20" s="19"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="14">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C21" s="14">
-        <v>268</v>
+        <v>192</v>
       </c>
       <c r="D21" s="15">
         <f>1000/C21</f>
-        <v>3.7313432835820897</v>
+        <v>5.208333333333333</v>
       </c>
       <c r="E21" s="16">
         <f>D21*C21</f>
@@ -2913,51 +3002,56 @@
         <v>22</v>
       </c>
       <c r="G21" s="17">
-        <v>42622</v>
+        <v>42625</v>
       </c>
       <c r="H21" s="18">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K21" s="27">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="L21" s="15">
-        <v>39.69</v>
+        <v>82</v>
       </c>
       <c r="M21" s="15">
         <f>((L21)/((K21*607.4)+157.9)*1000000)</f>
-        <v>178.40904442605463</v>
+        <v>385.43271167423978</v>
       </c>
       <c r="N21" s="15">
         <f>M21/4</f>
-        <v>44.602261106513659</v>
-      </c>
-      <c r="O21" s="17"/>
+        <v>96.358177918559946</v>
+      </c>
+      <c r="O21" s="18">
+        <v>3</v>
+      </c>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
       <c r="R21" s="14" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="14">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C22" s="14">
-        <v>392</v>
+        <v>256</v>
       </c>
       <c r="D22" s="15">
         <f>1000/C22</f>
-        <v>2.5510204081632653</v>
+        <v>3.90625</v>
       </c>
       <c r="E22" s="16">
         <f>D22*C22</f>
@@ -2967,50 +3061,53 @@
         <v>22</v>
       </c>
       <c r="G22" s="17">
-        <v>42622</v>
+        <v>42625</v>
       </c>
       <c r="H22" s="18">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K22" s="27">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="L22" s="15">
-        <v>16.190000000000001</v>
+        <v>3.81</v>
       </c>
       <c r="M22" s="15">
         <f>((L22)/((K22*607.4)+157.9)*1000000)</f>
-        <v>76.099458561048081</v>
+        <v>18.273723105612049</v>
       </c>
       <c r="N22" s="15">
         <f>M22/4</f>
-        <v>19.02486464026202</v>
+        <v>4.5684307764030123</v>
+      </c>
+      <c r="O22" s="18">
+        <v>3</v>
       </c>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="14">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C23" s="14">
-        <v>342</v>
+        <v>252</v>
       </c>
       <c r="D23" s="15">
         <f>1000/C23</f>
-        <v>2.9239766081871346</v>
+        <v>3.9682539682539684</v>
       </c>
       <c r="E23" s="16">
         <f>D23*C23</f>
@@ -3019,51 +3116,54 @@
       <c r="F23" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="17">
-        <v>42622</v>
+      <c r="G23" s="25">
+        <v>42621</v>
       </c>
       <c r="H23" s="18">
-        <v>18</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="K23" s="27">
-        <v>369</v>
+        <v>325</v>
       </c>
       <c r="L23" s="15">
-        <v>21.7</v>
+        <v>18.64</v>
       </c>
       <c r="M23" s="15">
         <f>((L23)/((K23*607.4)+157.9)*1000000)</f>
-        <v>96.750390679860971</v>
+        <v>94.349698248001019</v>
       </c>
       <c r="N23" s="15">
         <f>M23/4</f>
-        <v>24.187597669965243</v>
+        <v>23.587424562000255</v>
+      </c>
+      <c r="O23" s="18">
+        <v>4</v>
       </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="14">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C24" s="14">
-        <v>340</v>
+        <v>240</v>
       </c>
       <c r="D24" s="15">
         <f>1000/C24</f>
-        <v>2.9411764705882355</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="E24" s="16">
         <f>D24*C24</f>
@@ -3072,114 +3172,113 @@
       <c r="F24" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G24" s="17">
-        <v>42622</v>
+      <c r="G24" s="25">
+        <v>42621</v>
       </c>
       <c r="H24" s="18">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>31</v>
+        <v>161</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="K24" s="27">
-        <v>376</v>
+        <v>325</v>
       </c>
       <c r="L24" s="15">
-        <v>8.19</v>
+        <v>18.850000000000001</v>
       </c>
       <c r="M24" s="15">
         <f>((L24)/((K24*607.4)+157.9)*1000000)</f>
-        <v>35.836130433013352</v>
+        <v>95.412650857018207</v>
       </c>
       <c r="N24" s="15">
         <f>M24/4</f>
-        <v>8.959032608253338</v>
-      </c>
-      <c r="O24" s="17">
-        <v>42641</v>
-      </c>
-      <c r="P24" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>23.853162714254552</v>
+      </c>
+      <c r="O24" s="18">
+        <v>4</v>
+      </c>
+      <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="14">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C25" s="14">
-        <v>246</v>
+        <v>196</v>
       </c>
       <c r="D25" s="15">
         <f>1000/C25</f>
-        <v>4.0650406504065044</v>
+        <v>5.1020408163265305</v>
       </c>
       <c r="E25" s="16">
         <f>D25*C25</f>
-        <v>1000.0000000000001</v>
+        <v>1000</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="17">
-        <v>42622</v>
+      <c r="G25" s="25">
+        <v>42621</v>
       </c>
       <c r="H25" s="18">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>31</v>
+        <v>162</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="K25" s="27">
-        <v>368</v>
+        <v>325</v>
       </c>
       <c r="L25" s="15">
-        <v>12.23</v>
+        <v>20.02</v>
       </c>
       <c r="M25" s="15">
         <f>((L25)/((K25*607.4)+157.9)*1000000)</f>
-        <v>54.676054436427584</v>
+        <v>101.33481539297105</v>
       </c>
       <c r="N25" s="15">
         <f>M25/4</f>
-        <v>13.669013609106896</v>
-      </c>
-      <c r="O25" s="17">
-        <v>42641</v>
-      </c>
-      <c r="P25" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>25.333703848242763</v>
+      </c>
+      <c r="O25" s="18">
+        <v>4</v>
+      </c>
+      <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
       <c r="R25" s="14" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="14">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="14">
-        <v>136</v>
+        <v>362</v>
       </c>
       <c r="D26" s="15">
         <f>1000/C26</f>
-        <v>7.3529411764705879</v>
+        <v>2.7624309392265194</v>
       </c>
       <c r="E26" s="16">
         <f>D26*C26</f>
@@ -3192,33 +3291,35 @@
         <v>42625</v>
       </c>
       <c r="H26" s="18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I26" s="14" t="s">
         <v>171</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K26" s="27">
-        <v>326</v>
+        <v>383</v>
       </c>
       <c r="L26" s="15">
-        <v>15.14</v>
+        <v>34.909999999999997</v>
       </c>
       <c r="M26" s="15">
         <f>((L26)/((K26*607.4)+157.9)*1000000)</f>
-        <v>76.398935662912166</v>
+        <v>149.9621335947397</v>
       </c>
       <c r="N26" s="15">
         <f>M26/4</f>
-        <v>19.099733915728041</v>
-      </c>
-      <c r="O26" s="14"/>
+        <v>37.490533398684924</v>
+      </c>
+      <c r="O26" s="18">
+        <v>4</v>
+      </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
       <c r="R26" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S26" s="19"/>
       <c r="T26" s="19"/>
@@ -3226,21 +3327,20 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="14">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C27" s="14">
-        <v>362</v>
+        <v>11.8</v>
       </c>
       <c r="D27" s="15">
-        <f>1000/C27</f>
-        <v>2.7624309392265194</v>
+        <v>10</v>
       </c>
       <c r="E27" s="16">
         <f>D27*C27</f>
-        <v>1000</v>
+        <v>118</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>22</v>
@@ -3249,51 +3349,51 @@
         <v>42625</v>
       </c>
       <c r="H27" s="18">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="I27" s="14" t="s">
         <v>172</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K27" s="27">
-        <v>383</v>
+        <v>350</v>
       </c>
       <c r="L27" s="15">
-        <v>34.909999999999997</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="M27" s="15">
         <f>((L27)/((K27*607.4)+157.9)*1000000)</f>
-        <v>149.9621335947397</v>
+        <v>86.252320234418306</v>
       </c>
       <c r="N27" s="15">
         <f>M27/4</f>
-        <v>37.490533398684924</v>
-      </c>
-      <c r="O27" s="14"/>
+        <v>21.563080058604577</v>
+      </c>
+      <c r="O27" s="18">
+        <v>4</v>
+      </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
       <c r="R27" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S27" s="19"/>
-      <c r="T27" s="19"/>
-      <c r="U27" s="19"/>
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="14">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C28" s="14">
-        <v>192</v>
+        <v>280</v>
       </c>
       <c r="D28" s="15">
         <f>1000/C28</f>
-        <v>5.208333333333333</v>
+        <v>3.5714285714285716</v>
       </c>
       <c r="E28" s="16">
         <f>D28*C28</f>
@@ -3303,51 +3403,53 @@
         <v>22</v>
       </c>
       <c r="G28" s="17">
-        <v>42625</v>
+        <v>42626</v>
       </c>
       <c r="H28" s="18">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="K28" s="27">
-        <v>350</v>
+        <v>374</v>
       </c>
       <c r="L28" s="15">
-        <v>82</v>
+        <v>62.01</v>
       </c>
       <c r="M28" s="15">
         <f>((L28)/((K28*607.4)+157.9)*1000000)</f>
-        <v>385.43271167423978</v>
+        <v>272.7806603306712</v>
       </c>
       <c r="N28" s="15">
         <f>M28/4</f>
-        <v>96.358177918559946</v>
-      </c>
-      <c r="O28" s="14"/>
+        <v>68.195165082667799</v>
+      </c>
+      <c r="O28" s="18">
+        <v>4</v>
+      </c>
       <c r="P28" s="14"/>
       <c r="Q28" s="14"/>
       <c r="R28" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:21" s="19" customFormat="1">
       <c r="A29" s="14">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C29" s="14">
-        <v>256</v>
+        <v>382</v>
       </c>
       <c r="D29" s="15">
         <f>1000/C29</f>
-        <v>3.90625</v>
+        <v>2.6178010471204187</v>
       </c>
       <c r="E29" s="16">
         <f>D29*C29</f>
@@ -3357,263 +3459,271 @@
         <v>22</v>
       </c>
       <c r="G29" s="17">
-        <v>42625</v>
+        <v>42626</v>
       </c>
       <c r="H29" s="18">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K29" s="27">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="L29" s="15">
-        <v>3.81</v>
+        <v>152.71</v>
       </c>
       <c r="M29" s="15">
         <f>((L29)/((K29*607.4)+157.9)*1000000)</f>
-        <v>18.273723105612049</v>
+        <v>738.89349356643493</v>
       </c>
       <c r="N29" s="15">
         <f>M29/4</f>
-        <v>4.5684307764030123</v>
-      </c>
-      <c r="O29" s="14"/>
+        <v>184.72337339160873</v>
+      </c>
+      <c r="O29" s="18">
+        <v>4</v>
+      </c>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
       <c r="R29" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="14">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C30" s="14">
-        <v>11.8</v>
+        <v>142</v>
       </c>
       <c r="D30" s="15">
-        <v>10</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E30" s="16">
         <f>D30*C30</f>
-        <v>118</v>
+        <v>624.80000000000007</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="17">
-        <v>42625</v>
+      <c r="G30" s="25">
+        <v>42620</v>
       </c>
       <c r="H30" s="18">
-        <v>18</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>31</v>
+        <v>8</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="K30" s="27">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="L30" s="15">
-        <v>18.350000000000001</v>
+        <v>60.72</v>
       </c>
       <c r="M30" s="15">
         <f>((L30)/((K30*607.4)+157.9)*1000000)</f>
-        <v>86.252320234418306</v>
-      </c>
-      <c r="N30" s="15">
+        <v>279.81605504523742</v>
+      </c>
+      <c r="N30" s="28">
         <f>M30/4</f>
-        <v>21.563080058604577</v>
-      </c>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
+        <v>69.954013761309355</v>
+      </c>
+      <c r="O30" s="17">
+        <v>42641</v>
+      </c>
+      <c r="P30" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="Q30" s="14"/>
       <c r="R30" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="14">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C31" s="14">
-        <v>294</v>
+        <v>580</v>
       </c>
       <c r="D31" s="15">
-        <f>1000/C31</f>
-        <v>3.4013605442176869</v>
+        <v>1.72</v>
       </c>
       <c r="E31" s="16">
         <f>D31*C31</f>
-        <v>999.99999999999989</v>
+        <v>997.6</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="17">
-        <v>42625</v>
+      <c r="G31" s="25">
+        <v>42620</v>
       </c>
       <c r="H31" s="18">
-        <v>5</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="K31" s="27">
-        <v>350</v>
+        <v>379</v>
       </c>
       <c r="L31" s="15">
-        <v>45.06</v>
+        <v>29.62</v>
       </c>
       <c r="M31" s="15">
         <f>((L31)/((K31*607.4)+157.9)*1000000)</f>
-        <v>211.79997546391763</v>
-      </c>
-      <c r="N31" s="15">
+        <v>128.57995550491074</v>
+      </c>
+      <c r="N31" s="28">
         <f>M31/4</f>
-        <v>52.949993865979408</v>
-      </c>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
+        <v>32.144988876227686</v>
+      </c>
+      <c r="O31" s="17">
+        <v>42641</v>
+      </c>
+      <c r="P31" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="Q31" s="14"/>
       <c r="R31" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="32" spans="1:21" s="19" customFormat="1">
-      <c r="A32" s="19">
-        <v>31</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="19">
-        <v>352</v>
-      </c>
-      <c r="D32" s="31">
+      <c r="A32" s="14">
+        <v>15</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="14">
+        <v>224</v>
+      </c>
+      <c r="D32" s="15">
         <f>1000/C32</f>
-        <v>2.8409090909090908</v>
-      </c>
-      <c r="E32" s="32">
+        <v>4.4642857142857144</v>
+      </c>
+      <c r="E32" s="16">
         <f>D32*C32</f>
         <v>1000</v>
       </c>
-      <c r="F32" s="32" t="s">
+      <c r="F32" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="36">
-        <v>42625</v>
-      </c>
-      <c r="H32" s="29">
-        <v>4</v>
-      </c>
-      <c r="I32" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="J32" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="K32" s="35">
-        <v>350</v>
-      </c>
-      <c r="L32" s="31">
-        <v>45.18</v>
-      </c>
-      <c r="M32" s="31">
+      <c r="G32" s="25">
+        <v>42621</v>
+      </c>
+      <c r="H32" s="18">
+        <v>14</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="J32" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" s="27">
+        <v>325</v>
+      </c>
+      <c r="L32" s="15">
+        <v>19.32</v>
+      </c>
+      <c r="M32" s="15">
         <f>((L32)/((K32*607.4)+157.9)*1000000)</f>
-        <v>212.36402333466043</v>
-      </c>
-      <c r="N32" s="31">
+        <v>97.791640029580449</v>
+      </c>
+      <c r="N32" s="15">
         <f>M32/4</f>
-        <v>53.091005833665108</v>
-      </c>
-      <c r="O32" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R32" s="19" t="s">
-        <v>36</v>
+        <v>24.447910007395112</v>
+      </c>
+      <c r="O32" s="17">
+        <v>42641</v>
+      </c>
+      <c r="P32" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
       <c r="U32" s="7"/>
     </row>
     <row r="33" spans="1:21" s="19" customFormat="1">
-      <c r="A33" s="19">
-        <v>32</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="19">
-        <v>284</v>
-      </c>
-      <c r="D33" s="31">
+      <c r="A33" s="14">
+        <v>16</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="14">
+        <v>356</v>
+      </c>
+      <c r="D33" s="15">
         <f>1000/C33</f>
-        <v>3.5211267605633805</v>
-      </c>
-      <c r="E33" s="32">
+        <v>2.808988764044944</v>
+      </c>
+      <c r="E33" s="16">
         <f>D33*C33</f>
-        <v>1000</v>
-      </c>
-      <c r="F33" s="32" t="s">
+        <v>1000.0000000000001</v>
+      </c>
+      <c r="F33" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="36">
-        <v>42625</v>
-      </c>
-      <c r="H33" s="29">
-        <v>3</v>
-      </c>
-      <c r="I33" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="J33" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="K33" s="35">
-        <v>350</v>
-      </c>
-      <c r="L33" s="31">
-        <v>83.06</v>
-      </c>
-      <c r="M33" s="31">
+      <c r="G33" s="25">
+        <v>42621</v>
+      </c>
+      <c r="H33" s="18">
+        <v>18</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K33" s="27">
+        <v>325</v>
+      </c>
+      <c r="L33" s="15">
+        <v>15</v>
+      </c>
+      <c r="M33" s="15">
         <f>((L33)/((K33*607.4)+157.9)*1000000)</f>
-        <v>390.41513453246779</v>
-      </c>
-      <c r="N33" s="31">
+        <v>75.925186358369913</v>
+      </c>
+      <c r="N33" s="15">
         <f>M33/4</f>
-        <v>97.603783633116947</v>
-      </c>
-      <c r="O33" s="36">
-        <v>42655</v>
-      </c>
-      <c r="R33" s="19" t="s">
-        <v>36</v>
+        <v>18.981296589592478</v>
+      </c>
+      <c r="O33" s="17">
+        <v>42641</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
@@ -3621,253 +3731,250 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="14">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C34" s="14">
-        <v>272</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="D34" s="15">
-        <f>1000/C34</f>
-        <v>3.6764705882352939</v>
+        <v>5</v>
       </c>
       <c r="E34" s="16">
         <f>D34*C34</f>
-        <v>1000</v>
+        <v>51</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G34" s="17">
-        <v>42626</v>
+        <v>42622</v>
       </c>
       <c r="H34" s="18">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K34" s="27">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="L34" s="15">
-        <v>67.319999999999993</v>
+        <v>17</v>
       </c>
       <c r="M34" s="15">
         <f>((L34)/((K34*607.4)+157.9)*1000000)</f>
-        <v>286.19808461549258</v>
+        <v>75.386923384269764</v>
       </c>
       <c r="N34" s="15">
         <f>M34/4</f>
-        <v>71.549521153873144</v>
+        <v>18.846730846067441</v>
       </c>
       <c r="O34" s="17">
         <v>42641</v>
       </c>
       <c r="P34" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q34" s="14"/>
       <c r="R34" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="14">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C35" s="14">
-        <v>516</v>
+        <v>236</v>
       </c>
       <c r="D35" s="15">
         <f>1000/C35</f>
-        <v>1.9379844961240309</v>
+        <v>4.2372881355932206</v>
       </c>
       <c r="E35" s="16">
         <f>D35*C35</f>
-        <v>1000</v>
+        <v>1000.0000000000001</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="17">
-        <v>42626</v>
+        <v>42622</v>
       </c>
       <c r="H35" s="18">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K35" s="27">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="L35" s="15">
-        <v>19.61</v>
+        <v>24.46</v>
       </c>
       <c r="M35" s="15">
         <f>((L35)/((K35*607.4)+157.9)*1000000)</f>
-        <v>87.195898191118644</v>
+        <v>111.47098404816495</v>
       </c>
       <c r="N35" s="15">
         <f>M35/4</f>
-        <v>21.798974547779661</v>
+        <v>27.867746012041238</v>
       </c>
       <c r="O35" s="17">
         <v>42641</v>
       </c>
       <c r="P35" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q35" s="14"/>
       <c r="R35" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S35" s="19"/>
+        <v>35</v>
+      </c>
       <c r="T35" s="19"/>
       <c r="U35" s="19"/>
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="14">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C36" s="14">
-        <v>280</v>
+        <v>340</v>
       </c>
       <c r="D36" s="15">
         <f>1000/C36</f>
-        <v>3.5714285714285716</v>
+        <v>2.9411764705882355</v>
       </c>
       <c r="E36" s="16">
         <f>D36*C36</f>
-        <v>1000</v>
+        <v>1000.0000000000001</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G36" s="17">
-        <v>42626</v>
+        <v>42622</v>
       </c>
       <c r="H36" s="18">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="K36" s="27">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="L36" s="15">
-        <v>62.01</v>
+        <v>8.19</v>
       </c>
       <c r="M36" s="15">
         <f>((L36)/((K36*607.4)+157.9)*1000000)</f>
-        <v>272.7806603306712</v>
+        <v>35.836130433013352</v>
       </c>
       <c r="N36" s="15">
         <f>M36/4</f>
-        <v>68.195165082667799</v>
-      </c>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
+        <v>8.959032608253338</v>
+      </c>
+      <c r="O36" s="17">
+        <v>42641</v>
+      </c>
+      <c r="P36" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="Q36" s="14"/>
       <c r="R36" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19"/>
-      <c r="U36" s="19"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="14">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C37" s="14">
-        <v>382</v>
+        <v>246</v>
       </c>
       <c r="D37" s="15">
         <f>1000/C37</f>
-        <v>2.6178010471204187</v>
+        <v>4.0650406504065044</v>
       </c>
       <c r="E37" s="16">
         <f>D37*C37</f>
-        <v>1000</v>
+        <v>1000.0000000000001</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G37" s="17">
-        <v>42626</v>
+        <v>42622</v>
       </c>
       <c r="H37" s="18">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="J37" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K37" s="27">
-        <v>340</v>
+        <v>368</v>
       </c>
       <c r="L37" s="15">
-        <v>152.71</v>
+        <v>12.23</v>
       </c>
       <c r="M37" s="15">
         <f>((L37)/((K37*607.4)+157.9)*1000000)</f>
-        <v>738.89349356643493</v>
+        <v>54.676054436427584</v>
       </c>
       <c r="N37" s="15">
         <f>M37/4</f>
-        <v>184.72337339160873</v>
-      </c>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
+        <v>13.669013609106896</v>
+      </c>
+      <c r="O37" s="17">
+        <v>42641</v>
+      </c>
+      <c r="P37" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="Q37" s="14"/>
       <c r="R37" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="14">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C38" s="14">
-        <v>300</v>
+        <v>272</v>
       </c>
       <c r="D38" s="15">
         <f>1000/C38</f>
-        <v>3.3333333333333335</v>
+        <v>3.6764705882352939</v>
       </c>
       <c r="E38" s="16">
         <f>D38*C38</f>
@@ -3880,47 +3987,59 @@
         <v>42626</v>
       </c>
       <c r="H38" s="18">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="J38" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="K38" s="27"/>
-      <c r="L38" s="15"/>
+        <v>30</v>
+      </c>
+      <c r="K38" s="27">
+        <v>387</v>
+      </c>
+      <c r="L38" s="15">
+        <v>67.319999999999993</v>
+      </c>
       <c r="M38" s="15">
         <f>((L38)/((K38*607.4)+157.9)*1000000)</f>
-        <v>0</v>
+        <v>286.19808461549258</v>
       </c>
       <c r="N38" s="15">
         <f>M38/4</f>
-        <v>0</v>
-      </c>
-      <c r="P38" s="14"/>
+        <v>71.549521153873144</v>
+      </c>
+      <c r="O38" s="17">
+        <v>42641</v>
+      </c>
+      <c r="P38" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="Q38" s="14"/>
       <c r="R38" s="14" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
     </row>
     <row r="39" spans="1:21" s="19" customFormat="1">
       <c r="A39" s="14">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C39" s="14">
-        <v>290</v>
+        <v>516</v>
       </c>
       <c r="D39" s="15">
         <f>1000/C39</f>
-        <v>3.4482758620689653</v>
+        <v>1.9379844961240309</v>
       </c>
       <c r="E39" s="16">
         <f>D39*C39</f>
-        <v>999.99999999999989</v>
+        <v>1000</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>22</v>
@@ -3929,37 +4048,38 @@
         <v>42626</v>
       </c>
       <c r="H39" s="18">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="K39" s="27">
-        <v>326</v>
+        <v>370</v>
       </c>
       <c r="L39" s="15">
-        <v>29.92</v>
+        <v>19.61</v>
       </c>
       <c r="M39" s="15">
         <f>((L39)/((K39*607.4)+157.9)*1000000)</f>
-        <v>150.98125198377357</v>
+        <v>87.195898191118644</v>
       </c>
       <c r="N39" s="15">
         <f>M39/4</f>
-        <v>37.745312995943394</v>
-      </c>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
+        <v>21.798974547779661</v>
+      </c>
+      <c r="O39" s="17">
+        <v>42641</v>
+      </c>
+      <c r="P39" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="Q39" s="14"/>
       <c r="R39" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="7"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="40" spans="1:21">
       <c r="D40" s="9"/>
@@ -3968,19 +4088,20 @@
       <c r="G40" s="11"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
+      <c r="O40" s="12"/>
     </row>
     <row r="49" spans="6:6">
       <c r="F49" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:U49">
-    <sortCondition ref="A2:A49"/>
+    <sortCondition ref="O2:O49"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="63" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="61" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4007,13 +4128,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="28" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -4021,338 +4142,338 @@
     </row>
     <row r="2" spans="1:4" ht="30">
       <c r="A2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
       <c r="A3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
       <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
       <c r="A5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30">
       <c r="A6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
       <c r="A7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30">
       <c r="A8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30">
       <c r="A9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30">
       <c r="A10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30">
       <c r="A11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30">
       <c r="A12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30">
       <c r="A13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30">
       <c r="A14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30">
       <c r="A15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30">
       <c r="A16" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30">
       <c r="A17" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30">
       <c r="A18" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30">
       <c r="A19" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30">
       <c r="A20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30">
       <c r="A21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30">
       <c r="A22" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30">
       <c r="A23" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30">
       <c r="A24" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
       <c r="A25" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -4364,4 +4485,438 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30">
+      <c r="A1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="18">
+        <v>10</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="18">
+        <v>12</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="18">
+        <v>18</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="18">
+        <v>5</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="18">
+        <v>4</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="18">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="18">
+        <v>4</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" s="18">
+        <v>5</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" s="18">
+        <v>14</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="18">
+        <v>21</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" s="18">
+        <v>3</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" s="18">
+        <v>12</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="18">
+        <v>18</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17" s="18">
+        <v>7</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="18">
+        <v>14</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="18">
+        <v>8</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" s="18">
+        <v>10</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B21" s="18">
+        <v>2</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B22" s="18">
+        <v>3</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B23" s="18">
+        <v>11</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D23" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="B24" s="18">
+        <v>9</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="18">
+        <v>13</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="B26" s="18">
+        <v>6</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="B27" s="18">
+        <v>18</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D27" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" s="18">
+        <v>16</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" s="18">
+        <v>21</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D29" s="18">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bulk changes, re-analysis, and results for run 3
</commit_message>
<xml_diff>
--- a/data/RNAseq-cellline-master.xlsx
+++ b/data/RNAseq-cellline-master.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-460" windowWidth="23040" windowHeight="17280" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2020" yWindow="0" windowWidth="23040" windowHeight="17280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Library information" sheetId="1" r:id="rId1"/>
@@ -1264,7 +1264,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1277,6 +1277,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1415,7 +1417,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="64">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1446,6 +1448,7 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1476,6 +1479,7 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="11"/>
   </cellStyles>
@@ -1808,8 +1812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O29" sqref="A1:O29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24:O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1905,11 +1909,11 @@
         <v>212</v>
       </c>
       <c r="D2" s="15">
-        <f>1000/C2</f>
+        <f t="shared" ref="D2:D8" si="0">1000/C2</f>
         <v>4.716981132075472</v>
       </c>
       <c r="E2" s="16">
-        <f>D2*C2</f>
+        <f t="shared" ref="E2:E39" si="1">D2*C2</f>
         <v>1000.0000000000001</v>
       </c>
       <c r="F2" s="16" t="s">
@@ -1934,11 +1938,11 @@
         <v>21.74</v>
       </c>
       <c r="M2" s="15">
-        <f>((L2)/((K2*607.4)+157.9)*1000000)</f>
+        <f t="shared" ref="M2:M39" si="2">((L2)/((K2*607.4)+157.9)*1000000)</f>
         <v>110.04090342873079</v>
       </c>
       <c r="N2" s="15">
-        <f>M2/4</f>
+        <f t="shared" ref="N2:N39" si="3">M2/4</f>
         <v>27.510225857182697</v>
       </c>
       <c r="O2" s="18">
@@ -1961,11 +1965,11 @@
         <v>420</v>
       </c>
       <c r="D3" s="15">
-        <f>1000/C3</f>
+        <f t="shared" si="0"/>
         <v>2.3809523809523809</v>
       </c>
       <c r="E3" s="16">
-        <f>D3*C3</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F3" s="16" t="s">
@@ -1990,11 +1994,11 @@
         <v>17.61</v>
       </c>
       <c r="M3" s="15">
-        <f>((L3)/((K3*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>89.13616878472628</v>
       </c>
       <c r="N3" s="15">
-        <f>M3/4</f>
+        <f t="shared" si="3"/>
         <v>22.28404219618157</v>
       </c>
       <c r="O3" s="18">
@@ -2017,11 +2021,11 @@
         <v>342</v>
       </c>
       <c r="D4" s="15">
-        <f>1000/C4</f>
+        <f t="shared" si="0"/>
         <v>2.9239766081871346</v>
       </c>
       <c r="E4" s="16">
-        <f>D4*C4</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F4" s="16" t="s">
@@ -2046,11 +2050,11 @@
         <v>21.7</v>
       </c>
       <c r="M4" s="15">
-        <f>((L4)/((K4*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>96.750390679860971</v>
       </c>
       <c r="N4" s="15">
-        <f>M4/4</f>
+        <f t="shared" si="3"/>
         <v>24.187597669965243</v>
       </c>
       <c r="O4" s="18">
@@ -2076,11 +2080,11 @@
         <v>136</v>
       </c>
       <c r="D5" s="15">
-        <f>1000/C5</f>
+        <f t="shared" si="0"/>
         <v>7.3529411764705879</v>
       </c>
       <c r="E5" s="16">
-        <f>D5*C5</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F5" s="16" t="s">
@@ -2105,11 +2109,11 @@
         <v>15.14</v>
       </c>
       <c r="M5" s="15">
-        <f>((L5)/((K5*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>76.398935662912166</v>
       </c>
       <c r="N5" s="15">
-        <f>M5/4</f>
+        <f t="shared" si="3"/>
         <v>19.099733915728041</v>
       </c>
       <c r="O5" s="18">
@@ -2135,11 +2139,11 @@
         <v>294</v>
       </c>
       <c r="D6" s="15">
-        <f>1000/C6</f>
+        <f t="shared" si="0"/>
         <v>3.4013605442176869</v>
       </c>
       <c r="E6" s="16">
-        <f>D6*C6</f>
+        <f t="shared" si="1"/>
         <v>999.99999999999989</v>
       </c>
       <c r="F6" s="16" t="s">
@@ -2164,11 +2168,11 @@
         <v>45.06</v>
       </c>
       <c r="M6" s="15">
-        <f>((L6)/((K6*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>211.79997546391763</v>
       </c>
       <c r="N6" s="15">
-        <f>M6/4</f>
+        <f t="shared" si="3"/>
         <v>52.949993865979408</v>
       </c>
       <c r="O6" s="18">
@@ -2191,11 +2195,11 @@
         <v>352</v>
       </c>
       <c r="D7" s="15">
-        <f>1000/C7</f>
+        <f t="shared" si="0"/>
         <v>2.8409090909090908</v>
       </c>
       <c r="E7" s="16">
-        <f>D7*C7</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F7" s="16" t="s">
@@ -2220,11 +2224,11 @@
         <v>45.18</v>
       </c>
       <c r="M7" s="15">
-        <f>((L7)/((K7*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>212.36402333466043</v>
       </c>
       <c r="N7" s="15">
-        <f>M7/4</f>
+        <f t="shared" si="3"/>
         <v>53.091005833665108</v>
       </c>
       <c r="O7" s="18">
@@ -2250,11 +2254,11 @@
         <v>290</v>
       </c>
       <c r="D8" s="15">
-        <f>1000/C8</f>
+        <f t="shared" si="0"/>
         <v>3.4482758620689653</v>
       </c>
       <c r="E8" s="16">
-        <f>D8*C8</f>
+        <f t="shared" si="1"/>
         <v>999.99999999999989</v>
       </c>
       <c r="F8" s="16" t="s">
@@ -2279,11 +2283,11 @@
         <v>29.92</v>
       </c>
       <c r="M8" s="15">
-        <f>((L8)/((K8*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>150.98125198377357</v>
       </c>
       <c r="N8" s="15">
-        <f>M8/4</f>
+        <f t="shared" si="3"/>
         <v>37.745312995943394</v>
       </c>
       <c r="O8" s="18">
@@ -2312,7 +2316,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="16">
-        <f>D9*C9</f>
+        <f t="shared" si="1"/>
         <v>678</v>
       </c>
       <c r="F9" s="16" t="s">
@@ -2337,11 +2341,11 @@
         <v>54.6</v>
       </c>
       <c r="M9" s="15">
-        <f>((L9)/((K9*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>237.01774377340064</v>
       </c>
       <c r="N9" s="28">
-        <f>M9/4</f>
+        <f t="shared" si="3"/>
         <v>59.25443594335016</v>
       </c>
       <c r="O9" s="18">
@@ -2370,7 +2374,7 @@
         <v>4.3</v>
       </c>
       <c r="E10" s="16">
-        <f>D10*C10</f>
+        <f t="shared" si="1"/>
         <v>146.19999999999999</v>
       </c>
       <c r="F10" s="16" t="s">
@@ -2395,11 +2399,11 @@
         <v>41.84</v>
       </c>
       <c r="M10" s="15">
-        <f>((L10)/((K10*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>194.44412171346914</v>
       </c>
       <c r="N10" s="28">
-        <f>M10/4</f>
+        <f t="shared" si="3"/>
         <v>48.611030428367286</v>
       </c>
       <c r="O10" s="18">
@@ -2425,7 +2429,7 @@
         <v>3.38</v>
       </c>
       <c r="E11" s="16">
-        <f>D11*C11</f>
+        <f t="shared" si="1"/>
         <v>1000.48</v>
       </c>
       <c r="F11" s="16" t="s">
@@ -2450,11 +2454,11 @@
         <v>23</v>
       </c>
       <c r="M11" s="15">
-        <f>((L11)/((K11*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>105.40087849340901</v>
       </c>
       <c r="N11" s="28">
-        <f>M11/4</f>
+        <f t="shared" si="3"/>
         <v>26.350219623352253</v>
       </c>
       <c r="O11" s="18">
@@ -2480,7 +2484,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="16">
-        <f>D12*C12</f>
+        <f t="shared" si="1"/>
         <v>1232</v>
       </c>
       <c r="F12" s="16" t="s">
@@ -2505,11 +2509,11 @@
         <v>16.03</v>
       </c>
       <c r="M12" s="15">
-        <f>((L12)/((K12*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>72.650934242066768</v>
       </c>
       <c r="N12" s="28">
-        <f>M12/4</f>
+        <f t="shared" si="3"/>
         <v>18.162733560516692</v>
       </c>
       <c r="O12" s="18">
@@ -2539,7 +2543,7 @@
         <v>3.4722222222222223</v>
       </c>
       <c r="E13" s="16">
-        <f>D13*C13</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F13" s="16" t="s">
@@ -2564,11 +2568,11 @@
         <v>24.09</v>
       </c>
       <c r="M13" s="15">
-        <f>((L13)/((K13*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>121.93584929154208</v>
       </c>
       <c r="N13" s="15">
-        <f>M13/4</f>
+        <f t="shared" si="3"/>
         <v>30.483962322885521</v>
       </c>
       <c r="O13" s="18">
@@ -2598,7 +2602,7 @@
         <v>3.5211267605633805</v>
       </c>
       <c r="E14" s="16">
-        <f>D14*C14</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F14" s="16" t="s">
@@ -2623,11 +2627,11 @@
         <v>83.06</v>
       </c>
       <c r="M14" s="15">
-        <f>((L14)/((K14*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>390.41513453246779</v>
       </c>
       <c r="N14" s="15">
-        <f>M14/4</f>
+        <f t="shared" si="3"/>
         <v>97.603783633116947</v>
       </c>
       <c r="O14" s="18">
@@ -2657,7 +2661,7 @@
         <v>3.3333333333333335</v>
       </c>
       <c r="E15" s="16">
-        <f>D15*C15</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F15" s="16" t="s">
@@ -2682,11 +2686,11 @@
         <v>140</v>
       </c>
       <c r="M15" s="15">
-        <f>((L15)/((K15*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>658.05584919992157</v>
       </c>
       <c r="N15" s="15">
-        <f>M15/4</f>
+        <f t="shared" si="3"/>
         <v>164.51396229998039</v>
       </c>
       <c r="O15" s="18">
@@ -2712,7 +2716,7 @@
         <v>3.97</v>
       </c>
       <c r="E16" s="16">
-        <f>D16*C16</f>
+        <f t="shared" si="1"/>
         <v>1000.44</v>
       </c>
       <c r="F16" s="16" t="s">
@@ -2737,11 +2741,11 @@
         <v>23.27</v>
       </c>
       <c r="M16" s="15">
-        <f>((L16)/((K16*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>107.8388710238761</v>
       </c>
       <c r="N16" s="15">
-        <f>M16/4</f>
+        <f t="shared" si="3"/>
         <v>26.959717755969024</v>
       </c>
       <c r="O16" s="18">
@@ -2767,7 +2771,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="16">
-        <f>D17*C17</f>
+        <f t="shared" si="1"/>
         <v>325</v>
       </c>
       <c r="F17" s="16" t="s">
@@ -2792,11 +2796,11 @@
         <v>49.02</v>
       </c>
       <c r="M17" s="15">
-        <f>((L17)/((K17*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>216.79646297145604</v>
       </c>
       <c r="N17" s="28">
-        <f>M17/4</f>
+        <f t="shared" si="3"/>
         <v>54.199115742864009</v>
       </c>
       <c r="O17" s="18">
@@ -2822,11 +2826,11 @@
         <v>228</v>
       </c>
       <c r="D18" s="15">
-        <f>1000/C18</f>
+        <f t="shared" ref="D18:D26" si="4">1000/C18</f>
         <v>4.3859649122807021</v>
       </c>
       <c r="E18" s="16">
-        <f>D18*C18</f>
+        <f t="shared" si="1"/>
         <v>1000.0000000000001</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -2851,11 +2855,11 @@
         <v>54.58</v>
       </c>
       <c r="M18" s="15">
-        <f>((L18)/((K18*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>240.09624965083106</v>
       </c>
       <c r="N18" s="15">
-        <f>M18/4</f>
+        <f t="shared" si="3"/>
         <v>60.024062412707764</v>
       </c>
       <c r="O18" s="18">
@@ -2878,11 +2882,11 @@
         <v>268</v>
       </c>
       <c r="D19" s="15">
-        <f>1000/C19</f>
+        <f t="shared" si="4"/>
         <v>3.7313432835820897</v>
       </c>
       <c r="E19" s="16">
-        <f>D19*C19</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F19" s="16" t="s">
@@ -2907,11 +2911,11 @@
         <v>39.69</v>
       </c>
       <c r="M19" s="15">
-        <f>((L19)/((K19*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>178.40904442605463</v>
       </c>
       <c r="N19" s="15">
-        <f>M19/4</f>
+        <f t="shared" si="3"/>
         <v>44.602261106513659</v>
       </c>
       <c r="O19" s="18">
@@ -2935,11 +2939,11 @@
         <v>392</v>
       </c>
       <c r="D20" s="15">
-        <f>1000/C20</f>
+        <f t="shared" si="4"/>
         <v>2.5510204081632653</v>
       </c>
       <c r="E20" s="16">
-        <f>D20*C20</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F20" s="16" t="s">
@@ -2964,11 +2968,11 @@
         <v>16.190000000000001</v>
       </c>
       <c r="M20" s="15">
-        <f>((L20)/((K20*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>76.099458561048081</v>
       </c>
       <c r="N20" s="15">
-        <f>M20/4</f>
+        <f t="shared" si="3"/>
         <v>19.02486464026202</v>
       </c>
       <c r="O20" s="18">
@@ -2991,11 +2995,11 @@
         <v>192</v>
       </c>
       <c r="D21" s="15">
-        <f>1000/C21</f>
+        <f t="shared" si="4"/>
         <v>5.208333333333333</v>
       </c>
       <c r="E21" s="16">
-        <f>D21*C21</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F21" s="16" t="s">
@@ -3020,11 +3024,11 @@
         <v>82</v>
       </c>
       <c r="M21" s="15">
-        <f>((L21)/((K21*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>385.43271167423978</v>
       </c>
       <c r="N21" s="15">
-        <f>M21/4</f>
+        <f t="shared" si="3"/>
         <v>96.358177918559946</v>
       </c>
       <c r="O21" s="18">
@@ -3050,11 +3054,11 @@
         <v>256</v>
       </c>
       <c r="D22" s="15">
-        <f>1000/C22</f>
+        <f t="shared" si="4"/>
         <v>3.90625</v>
       </c>
       <c r="E22" s="16">
-        <f>D22*C22</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F22" s="16" t="s">
@@ -3079,11 +3083,11 @@
         <v>3.81</v>
       </c>
       <c r="M22" s="15">
-        <f>((L22)/((K22*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>18.273723105612049</v>
       </c>
       <c r="N22" s="15">
-        <f>M22/4</f>
+        <f t="shared" si="3"/>
         <v>4.5684307764030123</v>
       </c>
       <c r="O22" s="18">
@@ -3106,11 +3110,11 @@
         <v>252</v>
       </c>
       <c r="D23" s="15">
-        <f>1000/C23</f>
+        <f t="shared" si="4"/>
         <v>3.9682539682539684</v>
       </c>
       <c r="E23" s="16">
-        <f>D23*C23</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F23" s="16" t="s">
@@ -3135,15 +3139,15 @@
         <v>18.64</v>
       </c>
       <c r="M23" s="15">
-        <f>((L23)/((K23*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>94.349698248001019</v>
       </c>
       <c r="N23" s="15">
-        <f>M23/4</f>
+        <f t="shared" si="3"/>
         <v>23.587424562000255</v>
       </c>
-      <c r="O23" s="18">
-        <v>4</v>
+      <c r="O23" s="17">
+        <v>42679</v>
       </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -3162,11 +3166,11 @@
         <v>240</v>
       </c>
       <c r="D24" s="15">
-        <f>1000/C24</f>
+        <f t="shared" si="4"/>
         <v>4.166666666666667</v>
       </c>
       <c r="E24" s="16">
-        <f>D24*C24</f>
+        <f t="shared" si="1"/>
         <v>1000.0000000000001</v>
       </c>
       <c r="F24" s="16" t="s">
@@ -3191,15 +3195,15 @@
         <v>18.850000000000001</v>
       </c>
       <c r="M24" s="15">
-        <f>((L24)/((K24*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>95.412650857018207</v>
       </c>
       <c r="N24" s="15">
-        <f>M24/4</f>
+        <f t="shared" si="3"/>
         <v>23.853162714254552</v>
       </c>
-      <c r="O24" s="18">
-        <v>4</v>
+      <c r="O24" s="17">
+        <v>42679</v>
       </c>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -3218,11 +3222,11 @@
         <v>196</v>
       </c>
       <c r="D25" s="15">
-        <f>1000/C25</f>
+        <f t="shared" si="4"/>
         <v>5.1020408163265305</v>
       </c>
       <c r="E25" s="16">
-        <f>D25*C25</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F25" s="16" t="s">
@@ -3247,15 +3251,15 @@
         <v>20.02</v>
       </c>
       <c r="M25" s="15">
-        <f>((L25)/((K25*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>101.33481539297105</v>
       </c>
       <c r="N25" s="15">
-        <f>M25/4</f>
+        <f t="shared" si="3"/>
         <v>25.333703848242763</v>
       </c>
-      <c r="O25" s="18">
-        <v>4</v>
+      <c r="O25" s="17">
+        <v>42679</v>
       </c>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
@@ -3277,11 +3281,11 @@
         <v>362</v>
       </c>
       <c r="D26" s="15">
-        <f>1000/C26</f>
+        <f t="shared" si="4"/>
         <v>2.7624309392265194</v>
       </c>
       <c r="E26" s="16">
-        <f>D26*C26</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F26" s="16" t="s">
@@ -3306,15 +3310,15 @@
         <v>34.909999999999997</v>
       </c>
       <c r="M26" s="15">
-        <f>((L26)/((K26*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>149.9621335947397</v>
       </c>
       <c r="N26" s="15">
-        <f>M26/4</f>
+        <f t="shared" si="3"/>
         <v>37.490533398684924</v>
       </c>
-      <c r="O26" s="18">
-        <v>4</v>
+      <c r="O26" s="17">
+        <v>42679</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
@@ -3339,7 +3343,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="16">
-        <f>D27*C27</f>
+        <f t="shared" si="1"/>
         <v>118</v>
       </c>
       <c r="F27" s="16" t="s">
@@ -3364,15 +3368,15 @@
         <v>18.350000000000001</v>
       </c>
       <c r="M27" s="15">
-        <f>((L27)/((K27*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>86.252320234418306</v>
       </c>
       <c r="N27" s="15">
-        <f>M27/4</f>
+        <f t="shared" si="3"/>
         <v>21.563080058604577</v>
       </c>
-      <c r="O27" s="18">
-        <v>4</v>
+      <c r="O27" s="17">
+        <v>42679</v>
       </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
@@ -3396,7 +3400,7 @@
         <v>3.5714285714285716</v>
       </c>
       <c r="E28" s="16">
-        <f>D28*C28</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F28" s="16" t="s">
@@ -3421,15 +3425,15 @@
         <v>62.01</v>
       </c>
       <c r="M28" s="15">
-        <f>((L28)/((K28*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>272.7806603306712</v>
       </c>
       <c r="N28" s="15">
-        <f>M28/4</f>
+        <f t="shared" si="3"/>
         <v>68.195165082667799</v>
       </c>
-      <c r="O28" s="18">
-        <v>4</v>
+      <c r="O28" s="17">
+        <v>42679</v>
       </c>
       <c r="P28" s="14"/>
       <c r="Q28" s="14"/>
@@ -3452,7 +3456,7 @@
         <v>2.6178010471204187</v>
       </c>
       <c r="E29" s="16">
-        <f>D29*C29</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F29" s="16" t="s">
@@ -3477,15 +3481,15 @@
         <v>152.71</v>
       </c>
       <c r="M29" s="15">
-        <f>((L29)/((K29*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>738.89349356643493</v>
       </c>
       <c r="N29" s="15">
-        <f>M29/4</f>
+        <f t="shared" si="3"/>
         <v>184.72337339160873</v>
       </c>
-      <c r="O29" s="18">
-        <v>4</v>
+      <c r="O29" s="17">
+        <v>42679</v>
       </c>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
@@ -3507,7 +3511,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E30" s="16">
-        <f>D30*C30</f>
+        <f t="shared" si="1"/>
         <v>624.80000000000007</v>
       </c>
       <c r="F30" s="16" t="s">
@@ -3532,11 +3536,11 @@
         <v>60.72</v>
       </c>
       <c r="M30" s="15">
-        <f>((L30)/((K30*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>279.81605504523742</v>
       </c>
       <c r="N30" s="28">
-        <f>M30/4</f>
+        <f t="shared" si="3"/>
         <v>69.954013761309355</v>
       </c>
       <c r="O30" s="17">
@@ -3564,7 +3568,7 @@
         <v>1.72</v>
       </c>
       <c r="E31" s="16">
-        <f>D31*C31</f>
+        <f t="shared" si="1"/>
         <v>997.6</v>
       </c>
       <c r="F31" s="16" t="s">
@@ -3589,11 +3593,11 @@
         <v>29.62</v>
       </c>
       <c r="M31" s="15">
-        <f>((L31)/((K31*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>128.57995550491074</v>
       </c>
       <c r="N31" s="28">
-        <f>M31/4</f>
+        <f t="shared" si="3"/>
         <v>32.144988876227686</v>
       </c>
       <c r="O31" s="17">
@@ -3622,7 +3626,7 @@
         <v>4.4642857142857144</v>
       </c>
       <c r="E32" s="16">
-        <f>D32*C32</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F32" s="16" t="s">
@@ -3647,11 +3651,11 @@
         <v>19.32</v>
       </c>
       <c r="M32" s="15">
-        <f>((L32)/((K32*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>97.791640029580449</v>
       </c>
       <c r="N32" s="15">
-        <f>M32/4</f>
+        <f t="shared" si="3"/>
         <v>24.447910007395112</v>
       </c>
       <c r="O32" s="17">
@@ -3683,7 +3687,7 @@
         <v>2.808988764044944</v>
       </c>
       <c r="E33" s="16">
-        <f>D33*C33</f>
+        <f t="shared" si="1"/>
         <v>1000.0000000000001</v>
       </c>
       <c r="F33" s="16" t="s">
@@ -3708,11 +3712,11 @@
         <v>15</v>
       </c>
       <c r="M33" s="15">
-        <f>((L33)/((K33*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>75.925186358369913</v>
       </c>
       <c r="N33" s="15">
-        <f>M33/4</f>
+        <f t="shared" si="3"/>
         <v>18.981296589592478</v>
       </c>
       <c r="O33" s="17">
@@ -3743,7 +3747,7 @@
         <v>5</v>
       </c>
       <c r="E34" s="16">
-        <f>D34*C34</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="F34" s="16" t="s">
@@ -3768,11 +3772,11 @@
         <v>17</v>
       </c>
       <c r="M34" s="15">
-        <f>((L34)/((K34*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>75.386923384269764</v>
       </c>
       <c r="N34" s="15">
-        <f>M34/4</f>
+        <f t="shared" si="3"/>
         <v>18.846730846067441</v>
       </c>
       <c r="O34" s="17">
@@ -3801,7 +3805,7 @@
         <v>4.2372881355932206</v>
       </c>
       <c r="E35" s="16">
-        <f>D35*C35</f>
+        <f t="shared" si="1"/>
         <v>1000.0000000000001</v>
       </c>
       <c r="F35" s="16" t="s">
@@ -3826,11 +3830,11 @@
         <v>24.46</v>
       </c>
       <c r="M35" s="15">
-        <f>((L35)/((K35*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>111.47098404816495</v>
       </c>
       <c r="N35" s="15">
-        <f>M35/4</f>
+        <f t="shared" si="3"/>
         <v>27.867746012041238</v>
       </c>
       <c r="O35" s="17">
@@ -3861,7 +3865,7 @@
         <v>2.9411764705882355</v>
       </c>
       <c r="E36" s="16">
-        <f>D36*C36</f>
+        <f t="shared" si="1"/>
         <v>1000.0000000000001</v>
       </c>
       <c r="F36" s="16" t="s">
@@ -3886,11 +3890,11 @@
         <v>8.19</v>
       </c>
       <c r="M36" s="15">
-        <f>((L36)/((K36*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>35.836130433013352</v>
       </c>
       <c r="N36" s="15">
-        <f>M36/4</f>
+        <f t="shared" si="3"/>
         <v>8.959032608253338</v>
       </c>
       <c r="O36" s="17">
@@ -3919,7 +3923,7 @@
         <v>4.0650406504065044</v>
       </c>
       <c r="E37" s="16">
-        <f>D37*C37</f>
+        <f t="shared" si="1"/>
         <v>1000.0000000000001</v>
       </c>
       <c r="F37" s="16" t="s">
@@ -3944,11 +3948,11 @@
         <v>12.23</v>
       </c>
       <c r="M37" s="15">
-        <f>((L37)/((K37*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>54.676054436427584</v>
       </c>
       <c r="N37" s="15">
-        <f>M37/4</f>
+        <f t="shared" si="3"/>
         <v>13.669013609106896</v>
       </c>
       <c r="O37" s="17">
@@ -3977,7 +3981,7 @@
         <v>3.6764705882352939</v>
       </c>
       <c r="E38" s="16">
-        <f>D38*C38</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F38" s="16" t="s">
@@ -4002,11 +4006,11 @@
         <v>67.319999999999993</v>
       </c>
       <c r="M38" s="15">
-        <f>((L38)/((K38*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>286.19808461549258</v>
       </c>
       <c r="N38" s="15">
-        <f>M38/4</f>
+        <f t="shared" si="3"/>
         <v>71.549521153873144</v>
       </c>
       <c r="O38" s="17">
@@ -4038,7 +4042,7 @@
         <v>1.9379844961240309</v>
       </c>
       <c r="E39" s="16">
-        <f>D39*C39</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="F39" s="16" t="s">
@@ -4063,11 +4067,11 @@
         <v>19.61</v>
       </c>
       <c r="M39" s="15">
-        <f>((L39)/((K39*607.4)+157.9)*1000000)</f>
+        <f t="shared" si="2"/>
         <v>87.195898191118644</v>
       </c>
       <c r="N39" s="15">
-        <f>M39/4</f>
+        <f t="shared" si="3"/>
         <v>21.798974547779661</v>
       </c>
       <c r="O39" s="17">
@@ -4115,7 +4119,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4491,7 +4495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>